<commit_message>
Global Irminger mooring Deployment 2 cal and Ingest CSV
Reviewed calibration files and created ingest sheets. Made corrections
as necessary to reference designators.
</commit_message>
<xml_diff>
--- a/GI02HYPM/Omaha_Cal_Info_GI02HYPM_00002.xlsx
+++ b/GI02HYPM/Omaha_Cal_Info_GI02HYPM_00002.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\Ingest sheets\ingestion-csvs\GI02HYPM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8620" yWindow="3540" windowWidth="25440" windowHeight="13600"/>
+    <workbookView xWindow="8625" yWindow="3540" windowWidth="25440" windowHeight="13605" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -17,7 +22,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -162,24 +167,6 @@
   </si>
   <si>
     <t>GI02HYPM</t>
-  </si>
-  <si>
-    <r>
-      <t>GI02HYPM-RIS01-01-CTDMOG0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>39</t>
-    </r>
-  </si>
-  <si>
-    <t>GI02HYPM-RIS01-01-CTDMOG039</t>
   </si>
   <si>
     <r>
@@ -203,8 +190,17 @@
     </r>
   </si>
   <si>
+    <t>Not Deployed;  No Calibration Cofficient</t>
+  </si>
+  <si>
+    <t>GI02HYPM-RIM01-02-CTDMOG039</t>
+  </si>
+  <si>
+    <t>GI02HYPM-GP001-00-ENG000000</t>
+  </si>
+  <si>
     <r>
-      <t>GI02HYPM-</t>
+      <t>GI02HYPM-RIM01-02-CTDMOG0</t>
     </r>
     <r>
       <rPr>
@@ -214,40 +210,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>RIS01</t>
+      <t>39</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-00-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SIOENG</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>000</t>
-    </r>
-  </si>
-  <si>
-    <t>Not Deployed;  No Calibration Cofficient</t>
   </si>
 </sst>
 </file>
@@ -255,11 +219,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="36" x14ac:knownFonts="1">
     <font>
@@ -676,14 +640,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -801,7 +765,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -819,7 +783,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -846,7 +810,7 @@
     <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
@@ -879,7 +843,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -900,10 +864,10 @@
     <xf numFmtId="0" fontId="31" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="30" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="30" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="30" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="30" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -936,7 +900,7 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="57" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="34" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="34" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1087,12 +1051,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Read Me"/>
@@ -1397,29 +1364,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J10:J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="11" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.6640625" style="11" customWidth="1"/>
-    <col min="12" max="12" width="17.1640625" style="11" customWidth="1"/>
-    <col min="13" max="13" width="17.83203125" style="11" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="11"/>
+    <col min="1" max="1" width="16.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="11" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" style="11" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" style="11" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" style="11" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="12" customFormat="1" ht="36">
+    <row r="1" spans="1:13" s="12" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
@@ -1456,7 +1423,7 @@
       <c r="L1" s="42"/>
       <c r="M1" s="42"/>
     </row>
-    <row r="2" spans="1:13" s="23" customFormat="1">
+    <row r="2" spans="1:13" s="23" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>44</v>
       </c>
@@ -1483,7 +1450,7 @@
         <v>2667</v>
       </c>
       <c r="J2" s="43" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K2" s="46"/>
       <c r="L2" s="47">
@@ -1495,49 +1462,49 @@
         <v>-39.523483333333331</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="23" customFormat="1">
+    <row r="3" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D3" s="30"/>
       <c r="E3" s="31"/>
       <c r="F3" s="30"/>
     </row>
-    <row r="4" spans="1:13" customFormat="1"/>
-    <row r="5" spans="1:13" customFormat="1"/>
-    <row r="6" spans="1:13" customFormat="1"/>
-    <row r="7" spans="1:13" customFormat="1"/>
-    <row r="8" spans="1:13" customFormat="1"/>
-    <row r="9" spans="1:13" customFormat="1"/>
-    <row r="10" spans="1:13" customFormat="1"/>
-    <row r="11" spans="1:13" s="23" customFormat="1">
+    <row r="4" spans="1:13" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:13" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:13" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:13" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:13" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:13" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:13" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D11" s="30"/>
       <c r="E11" s="31"/>
       <c r="F11" s="30"/>
     </row>
-    <row r="12" spans="1:13" s="23" customFormat="1">
+    <row r="12" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D12" s="30"/>
       <c r="E12" s="31"/>
       <c r="F12" s="30"/>
     </row>
-    <row r="13" spans="1:13" s="23" customFormat="1">
+    <row r="13" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D13" s="30"/>
       <c r="E13" s="31"/>
       <c r="F13" s="30"/>
     </row>
-    <row r="14" spans="1:13" s="23" customFormat="1">
+    <row r="14" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="30"/>
       <c r="E14" s="31"/>
       <c r="F14" s="30"/>
     </row>
-    <row r="15" spans="1:13" s="23" customFormat="1">
+    <row r="15" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D15" s="30"/>
       <c r="E15" s="31"/>
       <c r="F15" s="30"/>
     </row>
-    <row r="16" spans="1:13" s="23" customFormat="1">
+    <row r="16" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="30"/>
       <c r="E16" s="31"/>
       <c r="F16" s="30"/>
     </row>
-    <row r="17" spans="4:6" s="23" customFormat="1">
+    <row r="17" spans="4:6" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D17" s="30"/>
       <c r="E17" s="31"/>
       <c r="F17" s="30"/>
@@ -1555,28 +1522,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="29.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="15" customWidth="1"/>
-    <col min="8" max="11" width="10.6640625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="3"/>
+    <col min="1" max="1" width="29.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="15" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="15" customWidth="1"/>
+    <col min="8" max="11" width="10.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="5" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="20" customFormat="1">
+    <row r="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1599,7 +1566,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="20" customFormat="1">
+    <row r="2" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28"/>
       <c r="B2" s="28"/>
       <c r="C2" s="29"/>
@@ -1608,7 +1575,7 @@
       <c r="F2" s="19"/>
       <c r="G2" s="21"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -1631,7 +1598,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
@@ -1653,7 +1620,7 @@
       </c>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -1664,7 +1631,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="34">
-        <f t="shared" ref="D5:D26" si="0">D4</f>
+        <f>D4</f>
         <v>2350</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -1675,7 +1642,7 @@
       </c>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -1686,7 +1653,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="34">
-        <f t="shared" si="0"/>
+        <f>D5</f>
         <v>2350</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -1697,7 +1664,7 @@
       </c>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -1708,7 +1675,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="34">
-        <f t="shared" si="0"/>
+        <f>D6</f>
         <v>2350</v>
       </c>
       <c r="E7" s="26" t="s">
@@ -1721,7 +1688,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
@@ -1732,7 +1699,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="34">
-        <f t="shared" si="0"/>
+        <f>D7</f>
         <v>2350</v>
       </c>
       <c r="E8" s="26" t="s">
@@ -1745,7 +1712,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
@@ -1756,7 +1723,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="34">
-        <f t="shared" si="0"/>
+        <f>D8</f>
         <v>2350</v>
       </c>
       <c r="E9" s="26" t="s">
@@ -1769,7 +1736,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -1780,7 +1747,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="34">
-        <f t="shared" si="0"/>
+        <f>D9</f>
         <v>2350</v>
       </c>
       <c r="E10" s="26" t="s">
@@ -1793,7 +1760,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="33"/>
       <c r="C11" s="5"/>
@@ -1802,7 +1769,7 @@
       <c r="F11" s="9"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -1826,7 +1793,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
@@ -1837,7 +1804,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="34">
-        <f t="shared" si="0"/>
+        <f>D12</f>
         <v>1106</v>
       </c>
       <c r="E13" s="14" t="s">
@@ -1848,7 +1815,7 @@
         <v>-39.523483333333331</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="33"/>
       <c r="C14" s="5"/>
@@ -1856,7 +1823,7 @@
       <c r="E14" s="14"/>
       <c r="F14" s="15"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -1877,7 +1844,7 @@
         <v>59.972749999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>33</v>
       </c>
@@ -1888,7 +1855,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="34">
-        <f t="shared" si="0"/>
+        <f>D15</f>
         <v>97</v>
       </c>
       <c r="E16" s="6" t="s">
@@ -1899,7 +1866,7 @@
         <v>-39.523483333333331</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="33"/>
       <c r="C17" s="5"/>
@@ -1907,7 +1874,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="15"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -1928,7 +1895,7 @@
         <v>59.972749999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
@@ -1939,7 +1906,7 @@
         <v>2</v>
       </c>
       <c r="D19" s="34">
-        <f t="shared" si="0"/>
+        <f>D18</f>
         <v>1025</v>
       </c>
       <c r="E19" s="14" t="s">
@@ -1950,7 +1917,7 @@
         <v>-39.523483333333331</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="33"/>
       <c r="C20" s="5"/>
@@ -1958,32 +1925,33 @@
       <c r="E20" s="14"/>
       <c r="F20" s="15"/>
     </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="35" t="s">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G21" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="H21" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="15">
-        <v>2</v>
-      </c>
-      <c r="D21" s="36"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="37" t="s">
+      <c r="I21" s="15">
+        <v>2</v>
+      </c>
+      <c r="J21" s="36"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G22" s="35"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="36"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="37"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="35"/>
-      <c r="B22" s="32"/>
-      <c r="D22" s="36"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="37"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="B23" s="32" t="s">
         <v>37</v>
@@ -2001,9 +1969,9 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B24" s="33" t="s">
         <v>37</v>
@@ -2012,7 +1980,7 @@
         <v>2</v>
       </c>
       <c r="D24" s="34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D24:D26" si="0">D23</f>
         <v>37-13439</v>
       </c>
       <c r="E24" s="8" t="s">
@@ -2023,9 +1991,9 @@
         <v>59.972749999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B25" s="33" t="s">
         <v>37</v>
@@ -2045,9 +2013,9 @@
         <v>-39.523483333333331</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B26" s="33" t="s">
         <v>37</v>
@@ -2066,7 +2034,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="38"/>
       <c r="B27" s="33"/>
       <c r="C27" s="5"/>
@@ -2074,8 +2042,8 @@
       <c r="E27" s="7"/>
       <c r="F27" s="15"/>
     </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="39" t="s">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B28" s="32" t="s">
@@ -2091,7 +2059,7 @@
       <c r="F28" s="40"/>
       <c r="G28" s="41"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="39"/>
       <c r="B29" s="32"/>
       <c r="C29" s="3"/>
@@ -2100,7 +2068,7 @@
       <c r="F29" s="40"/>
       <c r="G29" s="41"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="39" t="s">
         <v>36</v>
       </c>
@@ -2117,7 +2085,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G31" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Irminger and PAPA FLM and HYPM CAL sheets
corrected lat lon formats, lat lon formats must be individual numbers
pasted into a cell and not a link
</commit_message>
<xml_diff>
--- a/GI02HYPM/Omaha_Cal_Info_GI02HYPM_00002.xlsx
+++ b/GI02HYPM/Omaha_Cal_Info_GI02HYPM_00002.xlsx
@@ -177,6 +177,7 @@
         <sz val="10"/>
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>-</t>
     </r>
@@ -407,22 +408,26 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -444,12 +449,14 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1118,7 +1125,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1153,7 +1160,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1364,8 +1371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J10:J11"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1522,11 +1529,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
+      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1609,7 +1616,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="34">
-        <f>D3</f>
+        <f t="shared" ref="D4:D10" si="0">D3</f>
         <v>2350</v>
       </c>
       <c r="E4" s="6" t="s">
@@ -1631,7 +1638,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="34">
-        <f>D4</f>
+        <f t="shared" si="0"/>
         <v>2350</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -1653,7 +1660,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="34">
-        <f>D5</f>
+        <f t="shared" si="0"/>
         <v>2350</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -1675,7 +1682,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="34">
-        <f>D6</f>
+        <f t="shared" si="0"/>
         <v>2350</v>
       </c>
       <c r="E7" s="26" t="s">
@@ -1699,7 +1706,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="34">
-        <f>D7</f>
+        <f t="shared" si="0"/>
         <v>2350</v>
       </c>
       <c r="E8" s="26" t="s">
@@ -1723,7 +1730,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="34">
-        <f>D8</f>
+        <f t="shared" si="0"/>
         <v>2350</v>
       </c>
       <c r="E9" s="26" t="s">
@@ -1747,7 +1754,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="34">
-        <f>D9</f>
+        <f t="shared" si="0"/>
         <v>2350</v>
       </c>
       <c r="E10" s="26" t="s">
@@ -1785,8 +1792,7 @@
       <c r="E12" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="15">
-        <f>Moorings!L2</f>
+      <c r="F12" s="3">
         <v>59.972749999999998</v>
       </c>
       <c r="G12" s="15" t="s">
@@ -1811,7 +1817,6 @@
         <v>7</v>
       </c>
       <c r="F13" s="15">
-        <f>Moorings!M2</f>
         <v>-39.523483333333331</v>
       </c>
     </row>
@@ -1839,8 +1844,7 @@
       <c r="E15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="15">
-        <f>Moorings!L2</f>
+      <c r="F15" s="3">
         <v>59.972749999999998</v>
       </c>
     </row>
@@ -1862,7 +1866,6 @@
         <v>9</v>
       </c>
       <c r="F16" s="15">
-        <f>Moorings!M2</f>
         <v>-39.523483333333331</v>
       </c>
     </row>
@@ -1890,8 +1893,7 @@
       <c r="E18" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="15">
-        <f>Moorings!L2</f>
+      <c r="F18" s="3">
         <v>59.972749999999998</v>
       </c>
     </row>
@@ -1913,7 +1915,6 @@
         <v>7</v>
       </c>
       <c r="F19" s="15">
-        <f>Moorings!M2</f>
         <v>-39.523483333333331</v>
       </c>
     </row>
@@ -1980,14 +1981,13 @@
         <v>2</v>
       </c>
       <c r="D24" s="34" t="str">
-        <f t="shared" ref="D24:D26" si="0">D23</f>
+        <f t="shared" ref="D24:D26" si="1">D23</f>
         <v>37-13439</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F24" s="15">
-        <f>Moorings!L2</f>
+      <c r="F24" s="3">
         <v>59.972749999999998</v>
       </c>
     </row>
@@ -2002,14 +2002,13 @@
         <v>2</v>
       </c>
       <c r="D25" s="34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37-13439</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F25" s="15">
-        <f>Moorings!M2</f>
         <v>-39.523483333333331</v>
       </c>
     </row>
@@ -2024,7 +2023,7 @@
         <v>2</v>
       </c>
       <c r="D26" s="34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37-13439</v>
       </c>
       <c r="E26" s="56" t="s">
@@ -2087,6 +2086,9 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G31" s="3"/>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>